<commit_message>
Production Verification Scripts done
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data-Prod.xlsx
+++ b/KatalonData/Bootstrap/UM-Data-Prod.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476046\Documents\katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6DBBAB-8744-4479-AB8F-C514648A8AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{6C6DBBAB-8744-4479-AB8F-C514648A8AEF}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
+    <workbookView activeTab="3" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
-    <sheet name="FindUser" sheetId="7" r:id="rId2"/>
-    <sheet name="ModifyUser" sheetId="18" r:id="rId3"/>
-    <sheet name="ModifyUserPwd" sheetId="19" r:id="rId4"/>
-    <sheet name="AddDeleteRole" sheetId="16" r:id="rId5"/>
-    <sheet name="SearchRole" sheetId="17" r:id="rId6"/>
+    <sheet name="CreateUser" r:id="rId1" sheetId="1"/>
+    <sheet name="FindUser" r:id="rId2" sheetId="7"/>
+    <sheet name="ModifyUser" r:id="rId3" sheetId="18"/>
+    <sheet name="ModifyUserPwd" r:id="rId4" sheetId="19"/>
+    <sheet name="AddDeleteRole" r:id="rId5" sheetId="16"/>
+    <sheet name="SearchRole" r:id="rId6" sheetId="17"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="64">
   <si>
     <t>Result</t>
   </si>
@@ -139,12 +139,106 @@
   </si>
   <si>
     <t>Wed Dec 18 21:47:36 IST 2024</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Fri Feb 28 06:30:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Feb 28 06:31:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Feb 28 06:32:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Feb 28 06:33:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Feb 28 06:34:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Feb 28 06:35:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 05 23:44:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 05 23:45:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 05 23:45:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 05 23:46:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 05 23:47:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 05 23:48:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Mar 13 02:46:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Mar 13 02:47:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Mar 13 02:48:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Mar 13 02:49:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Mar 13 02:50:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Mar 13 02:51:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Mar 13 21:48:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Mar 13 21:49:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Mar 13 21:50:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Mar 13 21:51:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Mar 13 21:51:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Mar 13 21:52:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Mar 14 07:14:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Mar 14 07:15:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Mar 14 07:15:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Mar 14 07:16:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Mar 14 07:17:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Mar 14 07:18:19 IST 2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -187,21 +281,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -218,10 +312,10 @@
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -256,7 +350,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -308,7 +402,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -419,21 +513,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -450,7 +544,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -502,15 +596,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office 2013 - 2022 Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -518,18 +612,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.5546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.109375" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.6640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="14.109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.88671875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="26.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="23.5546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="29.109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.88671875" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -572,7 +666,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -601,8 +695,8 @@
       <c r="J4"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -610,8 +704,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -619,15 +713,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="19.33203125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.88671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="13.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.33203125" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="19.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -661,7 +755,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -714,8 +808,8 @@
       <c r="B13"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -723,8 +817,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28ECF6F8-94D7-41D5-B6FF-650248E68667}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28ECF6F8-94D7-41D5-B6FF-650248E68667}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:K2"/>
@@ -732,7 +826,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -772,7 +866,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -797,13 +891,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5380E685-D2A4-4DCA-A76F-EFBA3980BCE7}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5380E685-D2A4-4DCA-A76F-EFBA3980BCE7}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
@@ -811,9 +905,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.77734375" customWidth="1"/>
+    <col min="5" max="5" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="17.44140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="16.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -853,7 +947,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -872,13 +966,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A53983D-C89C-4548-8A02-C36CB8EC5C28}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A53983D-C89C-4548-8A02-C36CB8EC5C28}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -886,12 +980,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.88671875" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="9.109375" style="3" collapsed="1"/>
-    <col min="5" max="5" width="18.33203125" style="3" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21" style="3" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.109375" style="3" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="6.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="29.88671875" collapsed="true"/>
+    <col min="3" max="4" style="3" width="9.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="18.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="21.0" collapsed="true"/>
+    <col min="7" max="16384" style="3" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -919,7 +1013,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>11</v>
@@ -944,13 +1038,13 @@
       <c r="B5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCABF931-E9E5-40BE-B844-C9FC3C47A38B}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCABF931-E9E5-40BE-B844-C9FC3C47A38B}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:F5"/>
@@ -958,12 +1052,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3" collapsed="1"/>
-    <col min="2" max="2" width="22.6640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="9.109375" style="3" collapsed="1"/>
-    <col min="5" max="5" width="24" style="3" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.6640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.109375" style="3" collapsed="1"/>
+    <col min="1" max="1" style="3" width="9.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="22.6640625" collapsed="true"/>
+    <col min="3" max="4" style="3" width="9.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="24.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="22.6640625" collapsed="true"/>
+    <col min="7" max="16384" style="3" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -991,7 +1085,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>11</v>
@@ -1016,6 +1110,6 @@
       <c r="B5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Demo Verification Script and Display CF
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data-Prod.xlsx
+++ b/KatalonData/Bootstrap/UM-Data-Prod.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476046\Documents\katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{6C6DBBAB-8744-4479-AB8F-C514648A8AEF}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{9C6178B9-9506-4020-87A3-EC398755FDB3}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="-108"/>
+    <workbookView windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" r:id="rId1" sheetId="1"/>
@@ -40,20 +40,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="73">
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="70">
   <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Execute</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -108,21 +99,9 @@
     <t>MelancholyKrat</t>
   </si>
   <si>
-    <t>Wed Dec 11 19:53:09 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Dec 11 20:24:37 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Dec 11 20:38:14 IST 2024</t>
-  </si>
-  <si>
     <t>Roger</t>
   </si>
   <si>
-    <t>Fri Dec 13 19:56:49 IST 2024</t>
-  </si>
-  <si>
     <t>PasswordSpChar</t>
   </si>
   <si>
@@ -135,130 +114,142 @@
     <t>@Bb2</t>
   </si>
   <si>
-    <t>Tue Dec 17 19:56:15 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Dec 18 21:47:36 IST 2024</t>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Wed Mar 26 00:42:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 26 00:43:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Mar 26 00:44:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Mar 27 21:36:25 IST 2025</t>
+  </si>
+  <si>
+    <t>ResultProd</t>
+  </si>
+  <si>
+    <t>DateProd</t>
+  </si>
+  <si>
+    <t>ResultDemo</t>
+  </si>
+  <si>
+    <t>DateDemo</t>
+  </si>
+  <si>
+    <t>ExecuteProd</t>
+  </si>
+  <si>
+    <t>ExecuteDemo</t>
+  </si>
+  <si>
+    <t>Thu Apr 17 21:12:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Apr 17 21:16:18 IST 2025</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Fri Feb 28 06:30:54 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Feb 28 06:31:49 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Feb 28 06:32:35 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Feb 28 06:33:33 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Feb 28 06:34:15 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Feb 28 06:35:29 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Mar 05 23:44:11 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Mar 05 23:45:05 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Mar 05 23:45:52 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Mar 05 23:46:43 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Mar 05 23:47:28 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Mar 05 23:48:26 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Mar 13 02:46:46 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Mar 13 02:47:38 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Mar 13 02:48:24 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Mar 13 02:49:24 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Mar 13 02:50:13 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Mar 13 02:51:33 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Mar 13 21:48:45 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Mar 13 21:49:30 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Mar 13 21:50:08 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Mar 13 21:51:02 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Mar 13 21:51:45 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Mar 13 21:52:59 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Mar 14 07:14:12 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Mar 14 07:15:04 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Mar 14 07:15:49 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Mar 14 07:16:42 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Mar 14 07:17:22 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri Mar 14 07:18:19 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Mar 26 00:39:23 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Mar 26 00:40:20 IST 2025</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Wed Mar 26 00:41:09 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Mar 26 00:42:04 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Mar 26 00:43:22 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Mar 26 00:44:23 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Mar 26 19:10:18 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Mar 27 21:36:25 IST 2025</t>
+    <t>Thu Apr 17 21:26:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 00:01:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 00:03:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 00:08:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 00:09:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 00:09:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 00:10:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 00:11:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 00:12:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 01:29:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 01:29:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 01:29:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 01:30:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 01:31:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 01:31:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 18:49:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 18:50:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 18:55:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 18:56:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 18:56:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 21:45:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 21:46:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 21:46:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 21:47:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 21:48:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Apr 30 21:48:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 01 18:56:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 01 18:56:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 01 18:57:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 01 18:57:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 01 18:58:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 01 18:59:27 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -631,95 +622,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5546875" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.6640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.33203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="14.109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.88671875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="26.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="23.5546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="29.109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.88671875" collapsed="true"/>
-    <col min="12" max="16384" style="1" width="9.109375" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" style="1" width="26.6640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="14.109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="9.88671875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="9.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="26.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="23.5546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="29.109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.88671875" collapsed="true"/>
+    <col min="15" max="16384" style="1" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2"/>
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4"/>
       <c r="B4"/>
-      <c r="H4" s="2"/>
-      <c r="I4"/>
-      <c r="J4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="K4" s="2"/>
+      <c r="L4"/>
+      <c r="M4"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -732,107 +743,143 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5546875" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.88671875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.33203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="13.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="14.6640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.33203125" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="19.33203125" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" style="1" width="25.88671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="13.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="14.6640625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="11.33203125" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="19.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C2"/>
+      <c r="D2"/>
       <c r="F2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="B3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C3"/>
+      <c r="D3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4"/>
       <c r="B4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C4"/>
+      <c r="D4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5"/>
       <c r="B5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C5"/>
+      <c r="D5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7"/>
       <c r="B7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C7"/>
+      <c r="D7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8"/>
       <c r="B8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C8"/>
+      <c r="D8"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9"/>
       <c r="B9"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C9"/>
+      <c r="D9"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10"/>
       <c r="B10"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C10"/>
+      <c r="D10"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="B11"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C11"/>
+      <c r="D11"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12"/>
       <c r="B12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C12"/>
+      <c r="D12"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13"/>
       <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -845,76 +892,88 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28ECF6F8-94D7-41D5-B6FF-650248E68667}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -924,71 +983,84 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5380E685-D2A4-4DCA-A76F-EFBA3980BCE7}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="17.44140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="16.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.21875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="17.44140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2">
         <v>13</v>
       </c>
     </row>
@@ -999,70 +1071,92 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A53983D-C89C-4548-8A02-C36CB8EC5C28}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="6.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="29.88671875" collapsed="true"/>
-    <col min="3" max="4" style="3" width="9.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="18.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="21.0" collapsed="true"/>
-    <col min="7" max="16384" style="3" width="9.109375" collapsed="true"/>
+    <col min="2" max="4" customWidth="true" style="3" width="29.88671875" collapsed="true"/>
+    <col min="5" max="7" style="3" width="9.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="3" width="18.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="3" width="21.0" collapsed="true"/>
+    <col min="10" max="16384" style="3" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2"/>
       <c r="F2" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="B3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C3"/>
+      <c r="D3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4"/>
       <c r="B4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C4"/>
+      <c r="D4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5"/>
       <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1071,70 +1165,87 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCABF931-E9E5-40BE-B844-C9FC3C47A38B}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F5"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" style="3" width="9.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="22.6640625" collapsed="true"/>
-    <col min="3" max="4" style="3" width="9.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="24.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="22.6640625" collapsed="true"/>
-    <col min="7" max="16384" style="3" width="9.109375" collapsed="true"/>
+    <col min="2" max="4" customWidth="true" style="3" width="22.6640625" collapsed="true"/>
+    <col min="5" max="7" style="3" width="9.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="3" width="24.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="3" width="22.6640625" collapsed="true"/>
+    <col min="10" max="16384" style="3" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="C2"/>
+      <c r="D2"/>
       <c r="F2" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="B3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C3"/>
+      <c r="D3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4"/>
       <c r="B4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C4"/>
+      <c r="D4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5"/>
       <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Made fixes for Prod/Demo Verification Script and Display Convenience fees qa done for all versions
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data-Prod.xlsx
+++ b/KatalonData/Bootstrap/UM-Data-Prod.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="126">
   <si>
     <t>Notes</t>
   </si>
@@ -250,6 +250,174 @@
   </si>
   <si>
     <t>Thu May 01 18:59:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 07 20:22:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 07 20:24:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 07 20:31:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 07 20:32:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 07 20:32:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 07 20:33:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 07 20:34:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 07 20:35:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 07 20:36:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 07 20:36:39 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 07 20:37:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 07 20:38:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 07 20:39:09 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:01:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:02:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:03:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:04:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:05:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:05:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:06:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:07:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:08:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:09:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:10:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:11:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:13:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:14:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:15:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:16:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:16:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:18:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:19:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:20:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:40:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:41:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:41:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:42:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:43:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:47:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:47:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:48:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:49:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu May 15 21:49:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri May 16 01:22:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 21 02:01:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 21 02:03:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 21 02:06:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 21 02:13:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 21 02:18:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 21 02:24:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 21 14:15:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 21 14:15:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 21 14:17:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 21 14:17:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 21 14:18:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 21 14:19:00 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -692,10 +860,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>122</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -801,12 +969,14 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2"/>
       <c r="D2"/>
       <c r="F2" s="1" t="s">
         <v>8</v>
@@ -946,10 +1116,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>124</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
@@ -1040,10 +1213,13 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>69</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -1121,7 +1297,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -1215,7 +1391,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>121</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>

</xml_diff>

<commit_message>
Fixes for Demo Verification SCript and Demo/QA CF
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data-Prod.xlsx
+++ b/KatalonData/Bootstrap/UM-Data-Prod.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476046\Documents\katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{9C6178B9-9506-4020-87A3-EC398755FDB3}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{D9CD3562-BFBA-4014-8F2C-4F5DEE2A72E6}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="-108"/>
+    <workbookView activeTab="4" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" r:id="rId1" sheetId="1"/>
     <sheet name="FindUser" r:id="rId2" sheetId="7"/>
     <sheet name="ModifyUser" r:id="rId3" sheetId="18"/>
     <sheet name="ModifyUserPwd" r:id="rId4" sheetId="19"/>
-    <sheet name="AddDeleteRole" r:id="rId5" sheetId="16"/>
-    <sheet name="SearchRole" r:id="rId6" sheetId="17"/>
+    <sheet name="FindCaseUser" r:id="rId5" sheetId="20"/>
+    <sheet name="AddDeleteRole" r:id="rId6" sheetId="16"/>
+    <sheet name="SearchRole" r:id="rId7" sheetId="17"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="50">
   <si>
     <t>Notes</t>
   </si>
@@ -114,21 +115,6 @@
     <t>@Bb2</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Wed Mar 26 00:42:04 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Mar 26 00:43:22 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Mar 26 00:44:23 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Mar 27 21:36:25 IST 2025</t>
-  </si>
-  <si>
     <t>ResultProd</t>
   </si>
   <si>
@@ -147,277 +133,64 @@
     <t>ExecuteDemo</t>
   </si>
   <si>
-    <t>Thu Apr 17 21:12:51 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Apr 17 21:16:18 IST 2025</t>
+    <t>Wed May 21 14:15:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 21 14:15:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 21 14:17:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed May 21 14:18:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jun 13 19:50:36 IST 2025</t>
+  </si>
+  <si>
+    <t>UsernameProd</t>
+  </si>
+  <si>
+    <t>UsernameDemo</t>
+  </si>
+  <si>
+    <t>ToBeModUserDemo</t>
+  </si>
+  <si>
+    <t>Tue Jun 17 19:26:02 IST 2025</t>
+  </si>
+  <si>
+    <t>CASEuser</t>
+  </si>
+  <si>
+    <t>CASEuserDemo</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Thu Apr 17 21:26:35 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 00:01:13 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 00:03:38 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 00:08:53 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 00:09:25 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 00:09:56 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 00:10:37 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 00:11:53 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 00:12:20 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 01:29:01 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 01:29:27 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 01:29:50 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 01:30:18 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 01:31:20 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 01:31:44 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 18:49:18 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 18:50:33 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 18:55:50 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 18:56:19 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 18:56:47 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 21:45:16 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 21:46:05 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 21:46:35 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 21:47:03 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 21:48:01 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 21:48:30 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 01 18:56:05 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 01 18:56:57 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 01 18:57:24 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 01 18:57:48 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 01 18:58:57 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 01 18:59:27 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:22:42 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:24:08 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:31:56 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:32:22 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:32:46 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:33:36 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:34:25 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:35:14 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:36:03 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:36:39 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:37:31 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:38:21 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:39:09 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:01:40 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:02:36 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:03:23 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:04:12 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:05:02 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:05:56 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:06:45 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:07:33 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:08:21 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:09:33 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:10:45 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:11:57 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:13:17 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:14:17 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:15:08 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:16:02 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:16:57 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:18:15 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:19:31 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:20:46 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:40:28 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:41:05 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:41:38 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:42:28 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:43:21 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:47:19 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:47:50 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:48:16 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:49:05 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:49:36 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri May 16 01:22:53 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 02:01:38 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 02:03:55 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 02:06:46 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 02:13:08 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 02:18:11 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 02:24:34 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 14:15:11 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 14:15:57 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 14:17:20 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 14:17:54 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 14:18:25 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 14:19:00 IST 2025</t>
+    <t>Wed Jun 18 20:08:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jun 18 20:15:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 19 17:46:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 19 17:47:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 19 17:47:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 19 17:47:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 19 17:48:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jun 19 17:49:32 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -792,49 +565,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.6640625" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" style="1" width="26.6640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.33203125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
     <col min="7" max="7" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="14.109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="9.88671875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="9.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="1" width="26.6640625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="23.5546875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="29.109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.88671875" collapsed="true"/>
-    <col min="15" max="16384" style="1" width="9.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="9.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="29.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
+    <col min="15" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -858,12 +631,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -891,7 +664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
@@ -914,45 +687,45 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection sqref="A1:K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="19.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.88671875" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" style="1" width="25.88671875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.33203125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
     <col min="7" max="7" customWidth="true" style="1" width="8.0" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="13.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="14.6640625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="11.33203125" collapsed="true"/>
-    <col min="12" max="16384" style="1" width="19.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="11.28515625" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="19.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -967,15 +740,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row ht="30" r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D2"/>
       <c r="F2" s="1" t="s">
@@ -991,61 +764,61 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
       <c r="D5"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -1068,29 +841,32 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" customWidth="true" width="30.140625" collapsed="true"/>
+  </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row ht="45" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -1114,12 +890,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -1156,70 +932,74 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5380E685-D2A4-4DCA-A76F-EFBA3980BCE7}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="22.21875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="17.44140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="16.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -1230,13 +1010,16 @@
       <c r="H2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" t="s">
+      <c r="I2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" t="s">
         <v>13</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>13</v>
       </c>
     </row>
@@ -1246,6 +1029,91 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECF5EAC-3F98-4000-BEA2-335F903FE34F}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="9" customWidth="true" width="22.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row ht="30" r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row ht="30" r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A53983D-C89C-4548-8A02-C36CB8EC5C28}">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -1253,37 +1121,37 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="6.5546875" collapsed="true"/>
-    <col min="2" max="4" customWidth="true" style="3" width="29.88671875" collapsed="true"/>
-    <col min="5" max="7" style="3" width="9.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="3" width="18.33203125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
+    <col min="2" max="4" customWidth="true" style="3" width="29.85546875" collapsed="true"/>
+    <col min="5" max="7" style="3" width="9.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="3" width="18.28515625" collapsed="true"/>
     <col min="9" max="9" customWidth="true" style="3" width="21.0" collapsed="true"/>
-    <col min="10" max="16384" style="3" width="9.109375" collapsed="true"/>
+    <col min="10" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>16</v>
@@ -1292,12 +1160,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -1316,19 +1184,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
@@ -1339,7 +1207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCABF931-E9E5-40BE-B844-C9FC3C47A38B}">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -1347,37 +1215,37 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="9.109375" collapsed="true"/>
-    <col min="2" max="4" customWidth="true" style="3" width="22.6640625" collapsed="true"/>
-    <col min="5" max="7" style="3" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" style="3" width="9.140625" collapsed="true"/>
+    <col min="2" max="4" customWidth="true" style="3" width="22.7109375" collapsed="true"/>
+    <col min="5" max="7" style="3" width="9.140625" collapsed="true"/>
     <col min="8" max="8" customWidth="true" style="3" width="24.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="3" width="22.6640625" collapsed="true"/>
-    <col min="10" max="16384" style="3" width="9.109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="3" width="22.7109375" collapsed="true"/>
+    <col min="10" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>16</v>
@@ -1386,12 +1254,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>31</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -1405,19 +1273,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>

</xml_diff>

<commit_message>
IWP TestData, Demo Verification Script: Committing after Windows 11 update
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data-Prod.xlsx
+++ b/KatalonData/Bootstrap/UM-Data-Prod.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476046\Documents\katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476046\Documents\VPS-Katalon-feature-VRelay\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{9C6178B9-9506-4020-87A3-EC398755FDB3}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{02EE98D3-C38F-4988-A46C-5BB33F628014}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="-108"/>
+    <workbookView activeTab="6" firstSheet="2" windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" r:id="rId1" sheetId="1"/>
     <sheet name="FindUser" r:id="rId2" sheetId="7"/>
     <sheet name="ModifyUser" r:id="rId3" sheetId="18"/>
     <sheet name="ModifyUserPwd" r:id="rId4" sheetId="19"/>
-    <sheet name="AddDeleteRole" r:id="rId5" sheetId="16"/>
-    <sheet name="SearchRole" r:id="rId6" sheetId="17"/>
+    <sheet name="FindCaseUser" r:id="rId5" sheetId="20"/>
+    <sheet name="AddDeleteRole" r:id="rId6" sheetId="16"/>
+    <sheet name="SearchRole" r:id="rId7" sheetId="17"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="60">
   <si>
     <t>Notes</t>
   </si>
@@ -114,310 +115,112 @@
     <t>@Bb2</t>
   </si>
   <si>
+    <t>ResultProd</t>
+  </si>
+  <si>
+    <t>DateProd</t>
+  </si>
+  <si>
+    <t>ResultDemo</t>
+  </si>
+  <si>
+    <t>DateDemo</t>
+  </si>
+  <si>
+    <t>ExecuteProd</t>
+  </si>
+  <si>
+    <t>ExecuteDemo</t>
+  </si>
+  <si>
+    <t>UsernameProd</t>
+  </si>
+  <si>
+    <t>UsernameDemo</t>
+  </si>
+  <si>
+    <t>ToBeModUserDemo</t>
+  </si>
+  <si>
+    <t>CASEuser</t>
+  </si>
+  <si>
+    <t>CASEuserDemo</t>
+  </si>
+  <si>
     <t>Fail</t>
   </si>
   <si>
-    <t>Wed Mar 26 00:42:04 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Mar 26 00:43:22 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Mar 26 00:44:23 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Mar 27 21:36:25 IST 2025</t>
-  </si>
-  <si>
-    <t>ResultProd</t>
-  </si>
-  <si>
-    <t>DateProd</t>
-  </si>
-  <si>
-    <t>ResultDemo</t>
-  </si>
-  <si>
-    <t>DateDemo</t>
-  </si>
-  <si>
-    <t>ExecuteProd</t>
-  </si>
-  <si>
-    <t>ExecuteDemo</t>
-  </si>
-  <si>
-    <t>Thu Apr 17 21:12:51 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Apr 17 21:16:18 IST 2025</t>
+    <t>Mon Jul 28 19:18:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jul 28 19:18:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jul 28 19:18:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jul 28 19:18:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jul 28 19:18:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jul 28 19:18:52 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jul 31 19:43:25 IST 2025</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Thu Apr 17 21:26:35 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 00:01:13 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 00:03:38 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 00:08:53 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 00:09:25 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 00:09:56 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 00:10:37 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 00:11:53 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 00:12:20 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 01:29:01 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 01:29:27 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 01:29:50 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 01:30:18 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 01:31:20 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 01:31:44 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 18:49:18 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 18:50:33 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 18:55:50 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 18:56:19 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 18:56:47 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 21:45:16 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 21:46:05 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 21:46:35 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 21:47:03 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 21:48:01 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 21:48:30 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 01 18:56:05 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 01 18:56:57 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 01 18:57:24 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 01 18:57:48 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 01 18:58:57 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 01 18:59:27 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:22:42 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:24:08 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:31:56 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:32:22 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:32:46 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:33:36 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:34:25 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:35:14 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:36:03 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:36:39 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:37:31 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:38:21 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 07 20:39:09 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:01:40 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:02:36 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:03:23 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:04:12 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:05:02 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:05:56 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:06:45 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:07:33 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:08:21 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:09:33 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:10:45 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:11:57 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:13:17 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:14:17 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:15:08 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:16:02 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:16:57 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:18:15 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:19:31 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:20:46 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:40:28 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:41:05 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:41:38 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:42:28 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:43:21 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:47:19 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:47:50 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:48:16 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:49:05 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu May 15 21:49:36 IST 2025</t>
-  </si>
-  <si>
-    <t>Fri May 16 01:22:53 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 02:01:38 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 02:03:55 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 02:06:46 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 02:13:08 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 02:18:11 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 02:24:34 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 14:15:11 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 14:15:57 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 14:17:20 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 14:17:54 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 14:18:25 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed May 21 14:19:00 IST 2025</t>
+    <t>Thu Jul 31 19:51:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jul 31 19:54:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jul 31 19:59:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jul 31 20:09:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jul 31 20:11:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jul 31 20:14:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Jul 31 20:30:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 01 19:58:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 01 20:01:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 04 20:09:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 04 20:11:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 04 20:15:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 04 20:20:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 04 20:22:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 04 20:23:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 04 20:25:43 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -792,7 +595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -816,25 +619,25 @@
   <sheetData>
     <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -860,15 +663,17 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="D2"/>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
@@ -914,7 +719,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection sqref="A1:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -934,25 +739,25 @@
   <sheetData>
     <row ht="28.8" r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -969,15 +774,17 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2"/>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1069,28 +876,31 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" customWidth="true" width="30.109375" collapsed="true"/>
+  </cols>
   <sheetData>
     <row ht="28.8" r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -1116,13 +926,16 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
@@ -1156,70 +969,77 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5380E685-D2A4-4DCA-A76F-EFBA3980BCE7}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="22.21875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="17.44140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="16.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="17.44140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="16.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H1" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
+      <c r="D2" t="s">
+        <v>58</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -1230,13 +1050,16 @@
       <c r="H2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" t="s">
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s">
         <v>13</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>13</v>
       </c>
     </row>
@@ -1246,6 +1069,94 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECF5EAC-3F98-4000-BEA2-335F903FE34F}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="9" customWidth="true" width="22.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row ht="28.8" r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row ht="28.8" r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A53983D-C89C-4548-8A02-C36CB8EC5C28}">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -1265,25 +1176,25 @@
   <sheetData>
     <row ht="28.8" r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>16</v>
@@ -1294,15 +1205,17 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="D2"/>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
       <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1339,12 +1252,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCABF931-E9E5-40BE-B844-C9FC3C47A38B}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1359,25 +1272,25 @@
   <sheetData>
     <row ht="28.8" r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>16</v>
@@ -1388,14 +1301,21 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C2"/>
-      <c r="D2"/>
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
       <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="3" t="s">

</xml_diff>

<commit_message>
Demo Verification Script fixes
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data-Prod.xlsx
+++ b/KatalonData/Bootstrap/UM-Data-Prod.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="83">
   <si>
     <t>Notes</t>
   </si>
@@ -221,6 +221,75 @@
   </si>
   <si>
     <t>Mon Aug 04 20:25:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 08 00:21:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 08 00:21:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 08 00:22:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 08 00:23:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 08 00:23:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 08 00:24:34 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 08 00:25:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 12 01:31:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 12 01:31:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 12 01:32:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 12 01:33:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 12 01:33:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 12 01:34:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 12 01:35:17 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 12 19:10:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 12 19:13:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 12 19:18:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 12 19:21:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 12 19:24:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 12 19:47:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 12 19:52:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 12 19:57:02 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 12 21:40:54 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -672,7 +741,7 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
@@ -783,7 +852,7 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
@@ -935,7 +1004,7 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
@@ -1039,7 +1108,7 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -1130,7 +1199,7 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
@@ -1214,7 +1283,7 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>8</v>
@@ -1307,10 +1376,10 @@
         <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Fixes for VRelay and Upgrade Verification SCript
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data-Prod.xlsx
+++ b/KatalonData/Bootstrap/UM-Data-Prod.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="108">
   <si>
     <t>Notes</t>
   </si>
@@ -290,6 +290,81 @@
   </si>
   <si>
     <t>Tue Aug 12 21:40:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 22:55:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 22:56:28 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 22:56:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 22:57:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 22:58:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 22:58:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 22:59:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:23:23 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 22:32:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 22:32:48 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 22:33:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 22:33:57 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 22:34:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 22:35:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 22:40:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 22:41:13 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 22:42:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 22:43:16 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 19:29:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 19:34:51 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 19:42:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 19:53:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 19:55:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 20:03:36 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 25 20:05:26 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -732,16 +807,16 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
@@ -843,16 +918,16 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
@@ -995,16 +1070,16 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
@@ -1099,16 +1174,16 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -1193,13 +1268,13 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
@@ -1274,16 +1349,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>8</v>
@@ -1370,16 +1445,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Ran Prod Verification Script
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data-Prod.xlsx
+++ b/KatalonData/Bootstrap/UM-Data-Prod.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="132">
   <si>
     <t>Notes</t>
   </si>
@@ -365,6 +365,78 @@
   </si>
   <si>
     <t>Mon Aug 25 20:05:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 27 21:52:20 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 27 21:53:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 27 21:53:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 27 21:54:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 27 21:55:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 27 21:56:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 27 21:57:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 27 21:58:30 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 27 22:00:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 27 22:01:06 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 27 22:03:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 00:20:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 00:22:54 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 00:24:24 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 00:26:43 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 07:21:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 07:22:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 07:29:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 07:30:31 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 07:31:00 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 07:31:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 07:32:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 07:33:04 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 07:34:05 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -810,7 +882,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -921,7 +993,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -1073,7 +1145,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -1177,7 +1249,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -1268,7 +1340,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -1352,7 +1424,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -1448,7 +1520,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
BWP Object Repository and fixes for VRelay
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data-Prod.xlsx
+++ b/KatalonData/Bootstrap/UM-Data-Prod.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="139">
   <si>
     <t>Notes</t>
   </si>
@@ -437,6 +437,27 @@
   </si>
   <si>
     <t>Thu Aug 28 07:34:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 04 06:14:25 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 04 06:15:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 04 06:15:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 04 06:16:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 04 06:16:55 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 04 06:17:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Sep 04 06:18:44 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -882,7 +903,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -993,7 +1014,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -1145,7 +1166,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -1249,7 +1270,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -1340,7 +1361,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -1424,7 +1445,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -1520,7 +1541,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Added BWP Bootstrap files
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data-Prod.xlsx
+++ b/KatalonData/Bootstrap/UM-Data-Prod.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="160">
   <si>
     <t>Notes</t>
   </si>
@@ -458,6 +458,69 @@
   </si>
   <si>
     <t>Thu Sep 04 06:18:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 06 22:15:07 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 06 22:15:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 06 22:16:26 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 06 22:17:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 06 22:17:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 06 22:18:29 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Nov 06 22:19:50 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 00:59:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 00:59:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 01:00:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 01:01:21 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 01:01:56 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 01:02:41 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 01:03:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 16:09:18 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 16:09:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 16:10:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 16:11:08 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 16:11:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 16:12:33 IST 2025</t>
+  </si>
+  <si>
+    <t>Mon Nov 10 16:13:47 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -903,13 +966,13 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>141</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
@@ -1014,13 +1077,13 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>142</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
@@ -1166,13 +1229,13 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>143</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
@@ -1270,13 +1333,13 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>144</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -1361,13 +1424,13 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>145</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
@@ -1445,13 +1508,13 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>139</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>8</v>
@@ -1541,13 +1604,13 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>140</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>8</v>

</xml_diff>